<commit_message>
[java->qt] - update class doc
</commit_message>
<xml_diff>
--- a/doc/classes.xlsx
+++ b/doc/classes.xlsx
@@ -86,19 +86,31 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -128,12 +140,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -436,151 +454,153 @@
   <dimension ref="B2:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="3.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:6" ht="19.5">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>50</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>100</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>100</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>100</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>100</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <v>70</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="E8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="2">
-        <v>100</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="4">
+        <v>80</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="4" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>